<commit_message>
Actualización completa Nivel 2: Sistema educativo con quizzes, videos victoria/derrota, indicador numérico de recursos con animación, pantalla tutor inicial
</commit_message>
<xml_diff>
--- a/datos_recolectados.xlsx
+++ b/datos_recolectados.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,7 +437,7 @@
     <col width="7" customWidth="1" min="1" max="1"/>
     <col width="21" customWidth="1" min="2" max="2"/>
     <col width="30" customWidth="1" min="3" max="3"/>
-    <col width="41" customWidth="1" min="4" max="4"/>
+    <col width="50" customWidth="1" min="4" max="4"/>
     <col width="15" customWidth="1" min="5" max="5"/>
     <col width="18" customWidth="1" min="6" max="6"/>
     <col width="16" customWidth="1" min="7" max="7"/>
@@ -714,6 +714,196 @@
         <v>1</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>2</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2025-11-13 00:22:47</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>sintoma_resuelto</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Virus ransomware eliminado de x_virus.exe</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>2</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2025-11-13 00:22:47</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>archivo_infectado_detectado</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Archivo spy_tool.exe puesto en cuarentena (Virus: spyware)</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>2</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>2025-11-13 00:22:47</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>archivo_limpio_eliminado</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Error: kernel32.dll era un archivo limpio y fue eliminado</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>2</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>2025-11-13 00:22:47</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>archivo_infectado_detectado</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Archivo adware_bundle.exe puesto en cuarentena (Virus: adware)</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>2</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>2025-11-13 00:22:47</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>archivo_limpio_cuarentena</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Falso positivo: logfile.log era seguro pero fue puesto en cuarentena</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H12" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
cambios en la pantalla de selección de niveles
</commit_message>
<xml_diff>
--- a/datos_recolectados.xlsx
+++ b/datos_recolectados.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,7 +437,7 @@
     <col width="7" customWidth="1" min="1" max="1"/>
     <col width="21" customWidth="1" min="2" max="2"/>
     <col width="30" customWidth="1" min="3" max="3"/>
-    <col width="41" customWidth="1" min="4" max="4"/>
+    <col width="50" customWidth="1" min="4" max="4"/>
     <col width="15" customWidth="1" min="5" max="5"/>
     <col width="18" customWidth="1" min="6" max="6"/>
     <col width="16" customWidth="1" min="7" max="7"/>
@@ -714,6 +714,196 @@
         <v>1</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>2</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2025-11-13 00:22:47</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>sintoma_resuelto</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Virus ransomware eliminado de x_virus.exe</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>2</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2025-11-13 00:22:47</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>archivo_infectado_detectado</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Archivo spy_tool.exe puesto en cuarentena (Virus: spyware)</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>2</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>2025-11-13 00:22:47</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>archivo_limpio_eliminado</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Error: kernel32.dll era un archivo limpio y fue eliminado</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>2</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>2025-11-13 00:22:47</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>archivo_infectado_detectado</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Archivo adware_bundle.exe puesto en cuarentena (Virus: adware)</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>2</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>2025-11-13 00:22:47</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>archivo_limpio_cuarentena</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Falso positivo: logfile.log era seguro pero fue puesto en cuarentena</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H12" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>